<commit_message>
Updated the release locations
</commit_message>
<xml_diff>
--- a/chapters/theoretical/docs/model-scenarios.xlsx
+++ b/chapters/theoretical/docs/model-scenarios.xlsx
@@ -181,7 +181,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="98">
   <si>
     <t>diel</t>
   </si>
@@ -411,9 +411,6 @@
     <t>ovm-impl3</t>
   </si>
   <si>
-    <t>Chromis chromis</t>
-  </si>
-  <si>
     <t>The length of the run (one year) cannot be tested until I can get one years data into the simulation, but early tests show that 1 day with 900,000 larvae is equal to 100seconds</t>
   </si>
   <si>
@@ -466,6 +463,18 @@
   </si>
   <si>
     <t>longitude range</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abudefduf vaigiensis </t>
+  </si>
+  <si>
+    <t>Wellington &amp; Victor 1989</t>
+  </si>
+  <si>
+    <t>Murphy et al. (2007)</t>
+  </si>
+  <si>
+    <t>n/a</t>
   </si>
 </sst>
 </file>
@@ -989,43 +998,43 @@
         <v>71</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="13"/>
       <c r="B12" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="13"/>
       <c r="B13" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="13"/>
       <c r="B14" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="13"/>
       <c r="B15" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="13"/>
       <c r="B16" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="13"/>
       <c r="B17" s="12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -1050,7 +1059,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B21" s="14">
         <v>19</v>
@@ -1066,7 +1075,7 @@
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="102" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1108,10 +1117,10 @@
         <v>26</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E2">
-        <v>2500</v>
+        <v>4000</v>
       </c>
       <c r="F2">
         <v>7</v>
@@ -1131,10 +1140,10 @@
         <v>10</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E3">
-        <v>2500</v>
+        <v>4000</v>
       </c>
       <c r="F3">
         <v>7</v>
@@ -1154,10 +1163,10 @@
         <v>11</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E4">
-        <v>2500</v>
+        <v>4000</v>
       </c>
       <c r="F4">
         <v>7</v>
@@ -1177,10 +1186,10 @@
         <v>12</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E5">
-        <v>2500</v>
+        <v>4000</v>
       </c>
       <c r="F5">
         <v>7</v>
@@ -1200,10 +1209,10 @@
         <v>13</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E6">
-        <v>2500</v>
+        <v>4000</v>
       </c>
       <c r="F6">
         <v>7</v>
@@ -1223,10 +1232,10 @@
         <v>14</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E7">
-        <v>2500</v>
+        <v>4000</v>
       </c>
       <c r="F7">
         <v>7</v>
@@ -1246,10 +1255,10 @@
         <v>15</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E8">
-        <v>2500</v>
+        <v>4000</v>
       </c>
       <c r="F8">
         <v>7</v>
@@ -1269,10 +1278,10 @@
         <v>16</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E9">
-        <v>2500</v>
+        <v>4000</v>
       </c>
       <c r="F9">
         <v>7</v>
@@ -1292,10 +1301,10 @@
         <v>17</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E10">
-        <v>2500</v>
+        <v>4000</v>
       </c>
       <c r="F10">
         <v>7</v>
@@ -1315,10 +1324,10 @@
         <v>18</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E11">
-        <v>2500</v>
+        <v>4000</v>
       </c>
       <c r="F11">
         <v>7</v>
@@ -1338,10 +1347,10 @@
         <v>19</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E12">
-        <v>2500</v>
+        <v>4000</v>
       </c>
       <c r="F12">
         <v>7</v>
@@ -1361,10 +1370,10 @@
         <v>20</v>
       </c>
       <c r="D13">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E13">
-        <v>2500</v>
+        <v>4000</v>
       </c>
       <c r="F13">
         <v>7</v>
@@ -1384,10 +1393,10 @@
         <v>21</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E14">
-        <v>2500</v>
+        <v>4000</v>
       </c>
       <c r="F14">
         <v>7</v>
@@ -1407,10 +1416,10 @@
         <v>22</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E15">
-        <v>2500</v>
+        <v>4000</v>
       </c>
       <c r="F15">
         <v>7</v>
@@ -1430,10 +1439,10 @@
         <v>23</v>
       </c>
       <c r="D16">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E16">
-        <v>2500</v>
+        <v>4000</v>
       </c>
       <c r="F16">
         <v>7</v>
@@ -1453,10 +1462,10 @@
         <v>24</v>
       </c>
       <c r="D17">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E17">
-        <v>2500</v>
+        <v>4000</v>
       </c>
       <c r="F17">
         <v>7</v>
@@ -1476,10 +1485,10 @@
         <v>25</v>
       </c>
       <c r="D18">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E18">
-        <v>2500</v>
+        <v>4000</v>
       </c>
       <c r="F18">
         <v>7</v>
@@ -1503,7 +1512,7 @@
       <c r="D20" s="2"/>
       <c r="E20" s="2">
         <f>SUM(E2:E18)</f>
-        <v>42500</v>
+        <v>68000</v>
       </c>
       <c r="F20" s="2">
         <f>AVERAGE((F2:F18))</f>
@@ -1515,12 +1524,12 @@
       </c>
       <c r="H20" s="3">
         <f>E20*G20/F20</f>
-        <v>2216071.4285714286</v>
+        <v>3545714.2857142859</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -1534,7 +1543,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17:D19"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1564,7 +1573,10 @@
         <v>46</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>76</v>
+        <v>94</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -1572,7 +1584,7 @@
         <v>29</v>
       </c>
       <c r="B3" s="4">
-        <v>18</v>
+        <v>18.3</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -1580,7 +1592,7 @@
         <v>30</v>
       </c>
       <c r="B4" s="4">
-        <v>2</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -1614,6 +1626,9 @@
       <c r="B8" s="4">
         <v>8</v>
       </c>
+      <c r="C8" s="4" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
@@ -1628,7 +1643,7 @@
         <v>42</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>34</v>
+        <v>97</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -1705,7 +1720,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B20" s="4">
         <f>SUM(B17:B19)</f>
@@ -1764,7 +1779,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1788,7 +1803,7 @@
         <v>58</v>
       </c>
       <c r="B2">
-        <v>0.25</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -1809,12 +1824,12 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -1837,7 +1852,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>32</v>
@@ -1849,7 +1864,7 @@
         <v>34</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -1908,7 +1923,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>32</v>
@@ -1976,7 +1991,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>32</v>
@@ -2044,7 +2059,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>32</v>
@@ -2112,7 +2127,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>32</v>
@@ -2180,7 +2195,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>32</v>
@@ -2248,7 +2263,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>32</v>
@@ -2335,13 +2350,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>87</v>
-      </c>
       <c r="D1" s="14" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -2349,7 +2364,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -2357,7 +2372,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -2365,7 +2380,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated the reef list and added the swimming values for the pomacentrids
</commit_message>
<xml_diff>
--- a/chapters/theoretical/docs/model-scenarios.xlsx
+++ b/chapters/theoretical/docs/model-scenarios.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3880" yWindow="3140" windowWidth="28160" windowHeight="16880" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="5980" yWindow="1500" windowWidth="28160" windowHeight="16880" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="model-scenarios" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
     <author>Steven Hawes</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0">
+    <comment ref="C1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -61,7 +61,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H20" authorId="0">
+    <comment ref="I20" authorId="0">
       <text>
         <r>
           <rPr>
@@ -152,7 +152,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A16" authorId="0">
+    <comment ref="A17" authorId="0">
       <text>
         <r>
           <rPr>
@@ -181,7 +181,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="122">
   <si>
     <t>diel</t>
   </si>
@@ -475,6 +475,78 @@
   </si>
   <si>
     <t>n/a</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>NSW01</t>
+  </si>
+  <si>
+    <t>NSW02</t>
+  </si>
+  <si>
+    <t>NSW03</t>
+  </si>
+  <si>
+    <t>NSW04</t>
+  </si>
+  <si>
+    <t>NSW05</t>
+  </si>
+  <si>
+    <t>NSW06</t>
+  </si>
+  <si>
+    <t>NSW07</t>
+  </si>
+  <si>
+    <t>NSW08</t>
+  </si>
+  <si>
+    <t>NSW09</t>
+  </si>
+  <si>
+    <t>NSW10</t>
+  </si>
+  <si>
+    <t>NSW11</t>
+  </si>
+  <si>
+    <t>NSW12</t>
+  </si>
+  <si>
+    <t>NSW13</t>
+  </si>
+  <si>
+    <t>NSW14</t>
+  </si>
+  <si>
+    <t>NSW15</t>
+  </si>
+  <si>
+    <t>NSW16</t>
+  </si>
+  <si>
+    <t>NSW17</t>
+  </si>
+  <si>
+    <t>critical swimming speed</t>
+  </si>
+  <si>
+    <t>in situ potential</t>
+  </si>
+  <si>
+    <t>endurance</t>
+  </si>
+  <si>
+    <t>Leis and Fisher (2006)</t>
   </si>
 </sst>
 </file>
@@ -915,10 +987,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -927,41 +999,50 @@
     <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
         <v>63</v>
       </c>
       <c r="B1" s="10" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>64</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="7"/>
       <c r="B3" s="7" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="7"/>
       <c r="B4" s="7" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="7"/>
       <c r="B5" s="7" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
         <v>65</v>
       </c>
@@ -969,31 +1050,31 @@
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="8"/>
       <c r="B7" s="8" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="8"/>
       <c r="B8" s="8" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="8"/>
       <c r="B9" s="8" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="8"/>
       <c r="B10" s="8" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
         <v>71</v>
       </c>
@@ -1001,31 +1082,31 @@
         <v>78</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="13"/>
       <c r="B12" s="12" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="13"/>
       <c r="B13" s="12" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="13"/>
       <c r="B14" s="12" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="13"/>
       <c r="B15" s="12" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="13"/>
       <c r="B16" s="12" t="s">
         <v>83</v>
@@ -1072,462 +1153,517 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="102" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView zoomScale="102" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="1" max="2" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>26</v>
       </c>
-      <c r="D2">
+      <c r="B2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E2">
         <v>5</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>4000</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>7</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>365</v>
       </c>
-      <c r="H2" s="1">
+      <c r="I2" s="1">
         <v>40179</v>
       </c>
-      <c r="I2" s="1">
+      <c r="J2" s="1">
         <v>40543</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="D3">
+      <c r="B3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E3">
         <v>5</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>4000</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>7</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>365</v>
       </c>
-      <c r="H3" s="1">
+      <c r="I3" s="1">
         <v>40179</v>
       </c>
-      <c r="I3" s="1">
+      <c r="J3" s="1">
         <v>40543</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>11</v>
       </c>
-      <c r="D4">
+      <c r="B4" t="s">
+        <v>103</v>
+      </c>
+      <c r="E4">
         <v>5</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>4000</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>7</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>365</v>
       </c>
-      <c r="H4" s="1">
+      <c r="I4" s="1">
         <v>40179</v>
       </c>
-      <c r="I4" s="1">
+      <c r="J4" s="1">
         <v>40543</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>12</v>
       </c>
-      <c r="D5">
+      <c r="B5" t="s">
+        <v>104</v>
+      </c>
+      <c r="E5">
         <v>5</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>4000</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>7</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>365</v>
       </c>
-      <c r="H5" s="1">
+      <c r="I5" s="1">
         <v>40179</v>
       </c>
-      <c r="I5" s="1">
+      <c r="J5" s="1">
         <v>40543</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>13</v>
       </c>
-      <c r="D6">
+      <c r="B6" t="s">
+        <v>105</v>
+      </c>
+      <c r="E6">
         <v>5</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>4000</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>7</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>365</v>
       </c>
-      <c r="H6" s="1">
+      <c r="I6" s="1">
         <v>40179</v>
       </c>
-      <c r="I6" s="1">
+      <c r="J6" s="1">
         <v>40543</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>14</v>
       </c>
-      <c r="D7">
+      <c r="B7" t="s">
+        <v>106</v>
+      </c>
+      <c r="E7">
         <v>5</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>4000</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>7</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>365</v>
       </c>
-      <c r="H7" s="1">
+      <c r="I7" s="1">
         <v>40179</v>
       </c>
-      <c r="I7" s="1">
+      <c r="J7" s="1">
         <v>40543</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>15</v>
       </c>
-      <c r="D8">
+      <c r="B8" t="s">
+        <v>107</v>
+      </c>
+      <c r="E8">
         <v>5</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>4000</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>7</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>365</v>
       </c>
-      <c r="H8" s="1">
+      <c r="I8" s="1">
         <v>40179</v>
       </c>
-      <c r="I8" s="1">
+      <c r="J8" s="1">
         <v>40543</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>16</v>
       </c>
-      <c r="D9">
+      <c r="B9" t="s">
+        <v>108</v>
+      </c>
+      <c r="E9">
         <v>5</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>4000</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>7</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>365</v>
       </c>
-      <c r="H9" s="1">
+      <c r="I9" s="1">
         <v>40179</v>
       </c>
-      <c r="I9" s="1">
+      <c r="J9" s="1">
         <v>40543</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>17</v>
       </c>
-      <c r="D10">
+      <c r="B10" t="s">
+        <v>109</v>
+      </c>
+      <c r="E10">
         <v>5</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>4000</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>7</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>365</v>
       </c>
-      <c r="H10" s="1">
+      <c r="I10" s="1">
         <v>40179</v>
       </c>
-      <c r="I10" s="1">
+      <c r="J10" s="1">
         <v>40543</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>18</v>
       </c>
-      <c r="D11">
+      <c r="B11" t="s">
+        <v>110</v>
+      </c>
+      <c r="E11">
         <v>5</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>4000</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>7</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>365</v>
       </c>
-      <c r="H11" s="1">
+      <c r="I11" s="1">
         <v>40179</v>
       </c>
-      <c r="I11" s="1">
+      <c r="J11" s="1">
         <v>40543</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>19</v>
       </c>
-      <c r="D12">
+      <c r="B12" t="s">
+        <v>111</v>
+      </c>
+      <c r="E12">
         <v>5</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>4000</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>7</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>365</v>
       </c>
-      <c r="H12" s="1">
+      <c r="I12" s="1">
         <v>40179</v>
       </c>
-      <c r="I12" s="1">
+      <c r="J12" s="1">
         <v>40543</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>20</v>
       </c>
-      <c r="D13">
+      <c r="B13" t="s">
+        <v>112</v>
+      </c>
+      <c r="E13">
         <v>5</v>
       </c>
-      <c r="E13">
+      <c r="F13">
         <v>4000</v>
       </c>
-      <c r="F13">
+      <c r="G13">
         <v>7</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <v>365</v>
       </c>
-      <c r="H13" s="1">
+      <c r="I13" s="1">
         <v>40179</v>
       </c>
-      <c r="I13" s="1">
+      <c r="J13" s="1">
         <v>40543</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>21</v>
       </c>
-      <c r="D14">
+      <c r="B14" t="s">
+        <v>113</v>
+      </c>
+      <c r="E14">
         <v>5</v>
       </c>
-      <c r="E14">
+      <c r="F14">
         <v>4000</v>
       </c>
-      <c r="F14">
+      <c r="G14">
         <v>7</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <v>365</v>
       </c>
-      <c r="H14" s="1">
+      <c r="I14" s="1">
         <v>40179</v>
       </c>
-      <c r="I14" s="1">
+      <c r="J14" s="1">
         <v>40543</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>22</v>
       </c>
-      <c r="D15">
+      <c r="B15" t="s">
+        <v>114</v>
+      </c>
+      <c r="E15">
         <v>5</v>
       </c>
-      <c r="E15">
+      <c r="F15">
         <v>4000</v>
       </c>
-      <c r="F15">
+      <c r="G15">
         <v>7</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <v>365</v>
       </c>
-      <c r="H15" s="1">
+      <c r="I15" s="1">
         <v>40179</v>
       </c>
-      <c r="I15" s="1">
+      <c r="J15" s="1">
         <v>40543</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>23</v>
       </c>
-      <c r="D16">
+      <c r="B16" t="s">
+        <v>115</v>
+      </c>
+      <c r="E16">
         <v>5</v>
       </c>
-      <c r="E16">
+      <c r="F16">
         <v>4000</v>
       </c>
-      <c r="F16">
+      <c r="G16">
         <v>7</v>
       </c>
-      <c r="G16">
+      <c r="H16">
         <v>365</v>
       </c>
-      <c r="H16" s="1">
+      <c r="I16" s="1">
         <v>40179</v>
       </c>
-      <c r="I16" s="1">
+      <c r="J16" s="1">
         <v>40543</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>24</v>
       </c>
-      <c r="D17">
+      <c r="B17" t="s">
+        <v>116</v>
+      </c>
+      <c r="E17">
         <v>5</v>
       </c>
-      <c r="E17">
+      <c r="F17">
         <v>4000</v>
       </c>
-      <c r="F17">
+      <c r="G17">
         <v>7</v>
       </c>
-      <c r="G17">
+      <c r="H17">
         <v>365</v>
       </c>
-      <c r="H17" s="1">
+      <c r="I17" s="1">
         <v>40179</v>
       </c>
-      <c r="I17" s="1">
+      <c r="J17" s="1">
         <v>40543</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>25</v>
       </c>
-      <c r="D18">
+      <c r="B18" t="s">
+        <v>117</v>
+      </c>
+      <c r="E18">
         <v>5</v>
       </c>
-      <c r="E18">
+      <c r="F18">
         <v>4000</v>
       </c>
-      <c r="F18">
+      <c r="G18">
         <v>7</v>
       </c>
-      <c r="G18">
+      <c r="H18">
         <v>365</v>
       </c>
-      <c r="H18" s="1">
+      <c r="I18" s="1">
         <v>40179</v>
       </c>
-      <c r="I18" s="1">
+      <c r="J18" s="1">
         <v>40543</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
-      <c r="E20" s="2">
-        <f>SUM(E2:E18)</f>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2">
+        <f>SUM(F2:F18)</f>
         <v>68000</v>
       </c>
-      <c r="F20" s="2">
-        <f>AVERAGE((F2:F18))</f>
+      <c r="G20" s="2">
+        <f>AVERAGE((G2:G18))</f>
         <v>7</v>
       </c>
-      <c r="G20" s="2">
-        <f>AVERAGE(G2:G18)</f>
+      <c r="H20" s="2">
+        <f>AVERAGE(H2:H18)</f>
         <v>365</v>
       </c>
-      <c r="H20" s="3">
-        <f>E20*G20/F20</f>
+      <c r="I20" s="3">
+        <f>F20*H20/G20</f>
         <v>3545714.2857142859</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>76</v>
       </c>
@@ -1540,16 +1676,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.83203125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="14.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="10.83203125" style="4"/>
     <col min="5" max="5" width="14.5" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.83203125" style="4" bestFit="1" customWidth="1"/>
@@ -1557,7 +1693,7 @@
     <col min="8" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>40</v>
       </c>
@@ -1568,7 +1704,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>46</v>
       </c>
@@ -1579,7 +1715,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>29</v>
       </c>
@@ -1587,7 +1723,7 @@
         <v>18.3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>30</v>
       </c>
@@ -1595,7 +1731,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>31</v>
       </c>
@@ -1603,7 +1739,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>35</v>
       </c>
@@ -1611,7 +1747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>36</v>
       </c>
@@ -1619,7 +1755,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>37</v>
       </c>
@@ -1630,7 +1766,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>38</v>
       </c>
@@ -1638,7 +1774,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>42</v>
       </c>
@@ -1646,7 +1782,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>49</v>
       </c>
@@ -1654,7 +1790,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>51</v>
       </c>
@@ -1662,109 +1798,136 @@
         <v>52</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="6" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B13" s="4">
+        <v>0.46300000000000002</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="B14" s="4">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="B15" s="4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B17" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C17" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D17" s="5" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B17" s="4">
-        <v>0.4</v>
-      </c>
-      <c r="C17" s="4">
-        <v>0.35</v>
-      </c>
-      <c r="D17" s="4">
-        <v>0.05</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="B18" s="4">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="C18" s="4">
-        <v>0.5</v>
+        <v>0.35</v>
       </c>
       <c r="D18" s="4">
-        <v>0.85</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="C19" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="D19" s="4">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B19" s="4">
+      <c r="B20" s="4">
         <v>0.1</v>
       </c>
-      <c r="C19" s="4">
+      <c r="C20" s="4">
         <v>0.15</v>
       </c>
-      <c r="D19" s="4">
+      <c r="D20" s="4">
         <v>0.1</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B20" s="4">
-        <f>SUM(B17:B19)</f>
+      <c r="B21" s="4">
+        <f>SUM(B18:B20)</f>
         <v>1</v>
       </c>
-      <c r="C20" s="4">
-        <f t="shared" ref="C20:D20" si="0">SUM(C17:C19)</f>
+      <c r="C21" s="4">
+        <f t="shared" ref="C21:D21" si="0">SUM(C18:C20)</f>
         <v>1</v>
       </c>
-      <c r="D20" s="4">
+      <c r="D21" s="4">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="6" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B22" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C22" s="5" t="s">
         <v>57</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="B22" s="4">
-        <v>0.8</v>
-      </c>
-      <c r="C22" s="4">
-        <v>0.1</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B23" s="4">
+        <v>0.8</v>
+      </c>
+      <c r="C23" s="4">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B23" s="4">
+      <c r="B24" s="4">
         <v>0.2</v>
       </c>
-      <c r="C23" s="4">
+      <c r="C24" s="4">
         <v>0.9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated the sensory zone ability to 15 km and removed the codes
</commit_message>
<xml_diff>
--- a/chapters/theoretical/docs/model-scenarios.xlsx
+++ b/chapters/theoretical/docs/model-scenarios.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28615"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28702"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5980" yWindow="1500" windowWidth="28160" windowHeight="16880" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="27700" yWindow="2120" windowWidth="28160" windowHeight="16880" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="model-scenarios" sheetId="1" r:id="rId1"/>
@@ -181,7 +181,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="119">
   <si>
     <t>diel</t>
   </si>
@@ -333,15 +333,9 @@
     <t>olfactory-sense</t>
   </si>
   <si>
-    <t>5km</t>
-  </si>
-  <si>
     <t>settlement-sense</t>
   </si>
   <si>
-    <t>2km</t>
-  </si>
-  <si>
     <t>ovm matrix</t>
   </si>
   <si>
@@ -480,12 +474,6 @@
     <t>code</t>
   </si>
   <si>
-    <t>P</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
     <t>NSW01</t>
   </si>
   <si>
@@ -547,6 +535,9 @@
   </si>
   <si>
     <t>Leis and Fisher (2006)</t>
+  </si>
+  <si>
+    <t>15 km</t>
   </si>
 </sst>
 </file>
@@ -987,10 +978,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -999,148 +990,139 @@
     <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B1" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="C1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="C2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="7"/>
       <c r="B3" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="7"/>
       <c r="B4" s="7" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="7"/>
       <c r="B5" s="7" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="8"/>
       <c r="B7" s="8" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="8"/>
       <c r="B8" s="8" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="8"/>
       <c r="B9" s="8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="8"/>
       <c r="B10" s="8" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="13"/>
       <c r="B12" s="12" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="13"/>
       <c r="B13" s="12" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="13"/>
       <c r="B14" s="12" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="13"/>
       <c r="B15" s="12" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="13"/>
       <c r="B16" s="12" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="13"/>
       <c r="B17" s="12" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="9"/>
       <c r="B19" s="9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="9"/>
       <c r="B20" s="9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="14" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B21" s="14">
         <v>19</v>
@@ -1169,7 +1151,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>3</v>
@@ -1201,7 +1183,7 @@
         <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="E2">
         <v>5</v>
@@ -1227,7 +1209,7 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E3">
         <v>5</v>
@@ -1253,7 +1235,7 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="E4">
         <v>5</v>
@@ -1279,7 +1261,7 @@
         <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="E5">
         <v>5</v>
@@ -1305,7 +1287,7 @@
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="E6">
         <v>5</v>
@@ -1331,7 +1313,7 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E7">
         <v>5</v>
@@ -1357,7 +1339,7 @@
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E8">
         <v>5</v>
@@ -1383,7 +1365,7 @@
         <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="E9">
         <v>5</v>
@@ -1409,7 +1391,7 @@
         <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="E10">
         <v>5</v>
@@ -1435,7 +1417,7 @@
         <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E11">
         <v>5</v>
@@ -1461,7 +1443,7 @@
         <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E12">
         <v>5</v>
@@ -1487,7 +1469,7 @@
         <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="E13">
         <v>5</v>
@@ -1513,7 +1495,7 @@
         <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="E14">
         <v>5</v>
@@ -1539,7 +1521,7 @@
         <v>22</v>
       </c>
       <c r="B15" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="E15">
         <v>5</v>
@@ -1565,7 +1547,7 @@
         <v>23</v>
       </c>
       <c r="B16" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="E16">
         <v>5</v>
@@ -1591,7 +1573,7 @@
         <v>24</v>
       </c>
       <c r="B17" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E17">
         <v>5</v>
@@ -1617,7 +1599,7 @@
         <v>25</v>
       </c>
       <c r="B18" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E18">
         <v>5</v>
@@ -1665,7 +1647,7 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1678,8 +1660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1701,7 +1683,7 @@
         <v>41</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -1709,10 +1691,10 @@
         <v>46</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -1763,7 +1745,7 @@
         <v>8</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -1779,7 +1761,7 @@
         <v>42</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -1787,31 +1769,31 @@
         <v>49</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>50</v>
+        <v>118</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>52</v>
+        <v>118</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B13" s="4">
         <v>0.46300000000000002</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B14" s="4">
         <v>0.25</v>
@@ -1819,7 +1801,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B15" s="4">
         <v>0.5</v>
@@ -1827,7 +1809,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>32</v>
@@ -1855,7 +1837,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B19" s="4">
         <v>0.5</v>
@@ -1883,7 +1865,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B21" s="4">
         <f>SUM(B18:B20)</f>
@@ -1900,18 +1882,18 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C22" s="5" t="s">
         <v>55</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B23" s="4">
         <v>0.8</v>
@@ -1958,12 +1940,12 @@
         <v>41</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B2">
         <v>0.3</v>
@@ -1971,7 +1953,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B3">
         <v>1.4999999999999999E-2</v>
@@ -1979,20 +1961,20 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -2004,7 +1986,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
@@ -2015,7 +1997,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>32</v>
@@ -2027,7 +2009,7 @@
         <v>34</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -2058,7 +2040,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B3" s="4">
         <v>0.5</v>
@@ -2086,7 +2068,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>32</v>
@@ -2126,7 +2108,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B7" s="4">
         <v>0.65</v>
@@ -2154,7 +2136,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>32</v>
@@ -2194,7 +2176,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B11" s="4">
         <v>0.52500000000000002</v>
@@ -2222,7 +2204,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>32</v>
@@ -2262,7 +2244,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B15" s="4">
         <v>0.55000000000000004</v>
@@ -2290,7 +2272,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>32</v>
@@ -2330,7 +2312,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B19" s="4">
         <v>0.47499999999999998</v>
@@ -2358,7 +2340,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>32</v>
@@ -2398,7 +2380,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B23" s="4">
         <v>0.3</v>
@@ -2426,7 +2408,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>32</v>
@@ -2466,7 +2448,7 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B27" s="4">
         <v>0.45</v>
@@ -2513,13 +2495,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -2527,7 +2509,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -2535,7 +2517,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -2543,7 +2525,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tidied up the final model scenarios
</commit_message>
<xml_diff>
--- a/chapters/theoretical/docs/model-scenarios.xlsx
+++ b/chapters/theoretical/docs/model-scenarios.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28702"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28810"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steve/Documents/PhD/Thesis/chapters/theoretical/docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Steven/Documents/Thesis/chapters/theoretical/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="27700" yWindow="2120" windowWidth="28160" windowHeight="16880" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="model-scenarios" sheetId="1" r:id="rId1"/>
@@ -181,7 +181,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="120">
   <si>
     <t>diel</t>
   </si>
@@ -538,6 +538,9 @@
   </si>
   <si>
     <t>15 km</t>
+  </si>
+  <si>
+    <t>52+8</t>
   </si>
 </sst>
 </file>
@@ -1135,10 +1138,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:N22"/>
   <sheetViews>
-    <sheetView zoomScale="102" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" zoomScale="102" workbookViewId="0">
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1146,7 +1149,7 @@
     <col min="1" max="2" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -1178,7 +1181,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -1203,8 +1206,11 @@
       <c r="J2" s="1">
         <v>40543</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L2">
+        <v>208000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -1229,8 +1235,15 @@
       <c r="J3" s="1">
         <v>40543</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L3">
+        <v>208000</v>
+      </c>
+      <c r="N3">
+        <f>250000/4000</f>
+        <v>62.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -1255,8 +1268,14 @@
       <c r="J4" s="1">
         <v>40543</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L4">
+        <v>208000</v>
+      </c>
+      <c r="N4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -1281,8 +1300,15 @@
       <c r="J5" s="1">
         <v>40543</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L5">
+        <v>208000</v>
+      </c>
+      <c r="N5">
+        <f>62*4000</f>
+        <v>248000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -1307,8 +1333,11 @@
       <c r="J6" s="1">
         <v>40543</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L6">
+        <v>208000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -1333,8 +1362,11 @@
       <c r="J7" s="1">
         <v>40543</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L7">
+        <v>208000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -1359,8 +1391,11 @@
       <c r="J8" s="1">
         <v>40543</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L8">
+        <v>208000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -1385,8 +1420,11 @@
       <c r="J9" s="1">
         <v>40543</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L9">
+        <v>208000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -1411,8 +1449,11 @@
       <c r="J10" s="1">
         <v>40543</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L10">
+        <v>208000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -1437,8 +1478,11 @@
       <c r="J11" s="1">
         <v>40543</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L11">
+        <v>208000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -1463,8 +1507,11 @@
       <c r="J12" s="1">
         <v>40543</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L12">
+        <v>208000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -1489,8 +1536,11 @@
       <c r="J13" s="1">
         <v>40543</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L13">
+        <v>208000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -1515,8 +1565,11 @@
       <c r="J14" s="1">
         <v>40543</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L14">
+        <v>208000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -1541,8 +1594,11 @@
       <c r="J15" s="1">
         <v>40543</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L15">
+        <v>208000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -1567,8 +1623,11 @@
       <c r="J16" s="1">
         <v>40543</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L16">
+        <v>208000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -1593,8 +1652,11 @@
       <c r="J17" s="1">
         <v>40543</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L17">
+        <v>208000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -1619,8 +1681,11 @@
       <c r="J18" s="1">
         <v>40543</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L18">
+        <v>208000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>27</v>
       </c>
@@ -1644,8 +1709,12 @@
         <f>F20*H20/G20</f>
         <v>3545714.2857142859</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L20">
+        <f>SUM(L2:L18)</f>
+        <v>3536000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>74</v>
       </c>
@@ -1986,7 +2055,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fixed names of release regions
</commit_message>
<xml_diff>
--- a/chapters/theoretical/docs/model-scenarios.xlsx
+++ b/chapters/theoretical/docs/model-scenarios.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28810"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Steven/Documents/Thesis/chapters/theoretical/docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steve/Documents/PhD/Thesis/chapters/theoretical/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="20680" yWindow="5140" windowWidth="17420" windowHeight="15460" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="model-scenarios" sheetId="1" r:id="rId1"/>
@@ -181,7 +181,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="119">
   <si>
     <t>diel</t>
   </si>
@@ -258,9 +258,6 @@
     <t>eden</t>
   </si>
   <si>
-    <t>lord howe</t>
-  </si>
-  <si>
     <t>the tweed</t>
   </si>
   <si>
@@ -387,9 +384,6 @@
     <t>ovm-orientation</t>
   </si>
   <si>
-    <t>passive-orientation</t>
-  </si>
-  <si>
     <t>three</t>
   </si>
   <si>
@@ -541,6 +535,9 @@
   </si>
   <si>
     <t>52+8</t>
+  </si>
+  <si>
+    <t>ballina</t>
   </si>
 </sst>
 </file>
@@ -981,10 +978,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -995,18 +992,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -1018,7 +1015,7 @@
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="7"/>
       <c r="B4" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -1029,105 +1026,99 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>63</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="8"/>
       <c r="B7" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="8"/>
       <c r="B8" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="8"/>
       <c r="B9" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="13" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8" t="s">
-        <v>68</v>
+      <c r="B10" s="12" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="13" t="s">
-        <v>69</v>
-      </c>
+      <c r="A11" s="13"/>
       <c r="B11" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="13"/>
       <c r="B12" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="13"/>
       <c r="B13" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="13"/>
       <c r="B14" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="13"/>
       <c r="B15" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="13"/>
       <c r="B16" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="13"/>
-      <c r="B17" s="12" t="s">
-        <v>82</v>
+      <c r="A17" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="9" t="s">
+      <c r="A18" s="9"/>
+      <c r="B18" s="9" t="s">
         <v>70</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="9"/>
       <c r="B19" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="9"/>
-      <c r="B20" s="9" t="s">
+      <c r="A20" s="14" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="B21" s="14">
+      <c r="B20" s="14">
         <v>19</v>
       </c>
     </row>
@@ -1140,8 +1131,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="102" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+    <sheetView zoomScale="102" workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1154,7 +1145,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>3</v>
@@ -1172,7 +1163,7 @@
         <v>7</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>8</v>
@@ -1183,10 +1174,10 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E2">
         <v>5</v>
@@ -1215,7 +1206,7 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E3">
         <v>5</v>
@@ -1245,10 +1236,10 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>118</v>
       </c>
       <c r="B4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E4">
         <v>5</v>
@@ -1272,15 +1263,15 @@
         <v>208000</v>
       </c>
       <c r="N4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E5">
         <v>5</v>
@@ -1310,10 +1301,10 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E6">
         <v>5</v>
@@ -1339,10 +1330,10 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E7">
         <v>5</v>
@@ -1368,10 +1359,10 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E8">
         <v>5</v>
@@ -1397,10 +1388,10 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E9">
         <v>5</v>
@@ -1426,10 +1417,10 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E10">
         <v>5</v>
@@ -1455,10 +1446,10 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E11">
         <v>5</v>
@@ -1484,10 +1475,10 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E12">
         <v>5</v>
@@ -1513,10 +1504,10 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E13">
         <v>5</v>
@@ -1542,10 +1533,10 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E14">
         <v>5</v>
@@ -1571,10 +1562,10 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B15" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E15">
         <v>5</v>
@@ -1600,10 +1591,10 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E16">
         <v>5</v>
@@ -1629,10 +1620,10 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B17" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E17">
         <v>5</v>
@@ -1658,10 +1649,10 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B18" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E18">
         <v>5</v>
@@ -1687,7 +1678,7 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -1716,7 +1707,7 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1746,29 +1737,29 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>41</v>
-      </c>
       <c r="C1" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B3" s="4">
         <v>18.3</v>
@@ -1776,7 +1767,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B4" s="4">
         <v>1.5</v>
@@ -1784,15 +1775,15 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B6" s="4">
         <v>0</v>
@@ -1800,7 +1791,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B7" s="4">
         <v>5</v>
@@ -1808,18 +1799,18 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B8" s="4">
         <v>8</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B9" s="4">
         <v>0.5</v>
@@ -1827,42 +1818,42 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B13" s="4">
         <v>0.46300000000000002</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B14" s="4">
         <v>0.25</v>
@@ -1870,7 +1861,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B15" s="4">
         <v>0.5</v>
@@ -1878,21 +1869,21 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B17" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="D17" s="5" t="s">
         <v>33</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B18" s="4">
         <v>0.4</v>
@@ -1906,7 +1897,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B19" s="4">
         <v>0.5</v>
@@ -1920,7 +1911,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B20" s="4">
         <v>0.1</v>
@@ -1934,7 +1925,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B21" s="4">
         <f>SUM(B18:B20)</f>
@@ -1951,18 +1942,18 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="C22" s="5" t="s">
         <v>54</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B23" s="4">
         <v>0.8</v>
@@ -1973,7 +1964,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B24" s="4">
         <v>0.2</v>
@@ -2003,18 +1994,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>41</v>
-      </c>
       <c r="C1" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B2">
         <v>0.3</v>
@@ -2022,7 +2013,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B3">
         <v>1.4999999999999999E-2</v>
@@ -2030,20 +2021,20 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" t="s">
         <v>59</v>
-      </c>
-      <c r="B4" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -2055,8 +2046,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2066,24 +2057,24 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="I1" s="14" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B2" s="4">
         <v>0.4</v>
@@ -2109,7 +2100,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B3" s="4">
         <v>0.5</v>
@@ -2123,7 +2114,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B4" s="4">
         <v>0.1</v>
@@ -2137,21 +2128,21 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="D5" s="5" t="s">
         <v>33</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B6" s="4">
         <v>0.27500000000000002</v>
@@ -2177,7 +2168,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B7" s="4">
         <v>0.65</v>
@@ -2191,7 +2182,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B8" s="4">
         <v>7.4999999999999997E-2</v>
@@ -2205,21 +2196,21 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B9" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="D9" s="5" t="s">
         <v>33</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B10" s="4">
         <v>0.42499999999999999</v>
@@ -2245,7 +2236,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B11" s="4">
         <v>0.52500000000000002</v>
@@ -2259,7 +2250,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B12" s="4">
         <v>0.05</v>
@@ -2273,21 +2264,21 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B13" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="D13" s="5" t="s">
         <v>33</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B14" s="4">
         <v>0.15</v>
@@ -2313,7 +2304,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B15" s="4">
         <v>0.55000000000000004</v>
@@ -2327,7 +2318,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B16" s="4">
         <v>0.3</v>
@@ -2341,21 +2332,21 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B17" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="D17" s="5" t="s">
         <v>33</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B18" s="4">
         <v>0.5</v>
@@ -2381,7 +2372,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B19" s="4">
         <v>0.47499999999999998</v>
@@ -2395,7 +2386,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B20" s="4">
         <v>2.5000000000000001E-2</v>
@@ -2409,21 +2400,21 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B21" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="D21" s="5" t="s">
         <v>33</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B22" s="4">
         <v>0.6</v>
@@ -2449,7 +2440,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B23" s="4">
         <v>0.3</v>
@@ -2463,7 +2454,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B24" s="4">
         <v>0.1</v>
@@ -2477,21 +2468,21 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B25" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="D25" s="5" t="s">
         <v>33</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B26" s="4">
         <v>0.45</v>
@@ -2517,7 +2508,7 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B27" s="4">
         <v>0.45</v>
@@ -2531,7 +2522,7 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B28" s="4">
         <v>0.1</v>
@@ -2552,8 +2543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2564,13 +2555,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -2578,7 +2569,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -2586,7 +2577,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -2594,7 +2585,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>